<commit_message>
ajout de page de deconnexion si besoin, probablement enlever si innutile
</commit_message>
<xml_diff>
--- a/journal de bord.xlsx
+++ b/journal de bord.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>commencer rfepartition tache</t>
   </si>
   <si>
-    <t>commencer compreention matos</t>
-  </si>
-  <si>
     <t>creation BDD sans valeur</t>
   </si>
   <si>
@@ -40,6 +37,15 @@
   </si>
   <si>
     <t>difficulté trouver but du mini projet</t>
+  </si>
+  <si>
+    <t>révision de la BDD &amp; ajout de quelque valeurs</t>
+  </si>
+  <si>
+    <t>connexion a la BDD faites dans l'index</t>
+  </si>
+  <si>
+    <t>commencer comprention matos</t>
   </si>
 </sst>
 </file>
@@ -372,55 +378,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1">
         <v>44473</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1">
+        <v>44474</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fin de l'heure, commit du projet, connexion OK mais classe nettoyage encore mal adapté et page web mal connecté si ce n'est pas connecté
</commit_message>
<xml_diff>
--- a/journal de bord.xlsx
+++ b/journal de bord.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>commencer rfepartition tache</t>
   </si>
@@ -42,10 +42,22 @@
     <t>révision de la BDD &amp; ajout de quelque valeurs</t>
   </si>
   <si>
-    <t>connexion a la BDD faites dans l'index</t>
-  </si>
-  <si>
     <t>commencer comprention matos</t>
+  </si>
+  <si>
+    <t>connexion a la BDD faites dans l'index (possiblement a deplacer)</t>
+  </si>
+  <si>
+    <t>que linterface donner ?</t>
+  </si>
+  <si>
+    <t>automatisation de la connexion</t>
+  </si>
+  <si>
+    <t>mis le projet sur GIT</t>
+  </si>
+  <si>
+    <t>gant complété</t>
   </si>
 </sst>
 </file>
@@ -418,18 +430,29 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
         <v>2</v>
       </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
@@ -437,6 +460,9 @@
       </c>
       <c r="B7" t="s">
         <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
l'API rest j'ai commencé a reflechir, nettoyage a modifier mais possiblement pas utile
</commit_message>
<xml_diff>
--- a/journal de bord.xlsx
+++ b/journal de bord.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>commencer rfepartition tache</t>
   </si>
@@ -58,6 +58,30 @@
   </si>
   <si>
     <t>gant complété</t>
+  </si>
+  <si>
+    <t>Ajout de liens a la BDD et rerévision</t>
+  </si>
+  <si>
+    <t>commencement a intégrer un formlaire connexion &amp; inscription</t>
+  </si>
+  <si>
+    <t>API rest en reflexion &amp; non fonctionnel</t>
+  </si>
+  <si>
+    <t>que mettre dans l'API rest</t>
+  </si>
+  <si>
+    <t>des liens dans la BDD difficile a comprendre</t>
+  </si>
+  <si>
+    <t>idcompte champ de tableau invalide (liens mal fait)</t>
+  </si>
+  <si>
+    <t>page inscription/connexion fonctionnel</t>
+  </si>
+  <si>
+    <t>page de planning fonctionnel</t>
   </si>
 </sst>
 </file>
@@ -390,20 +414,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="58.140625" customWidth="1"/>
+    <col min="4" max="4" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -413,8 +438,11 @@
       <c r="C1" s="1">
         <v>44474</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1">
+        <v>44475</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -424,37 +452,52 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="C6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -463,6 +506,19 @@
       </c>
       <c r="C7" t="s">
         <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="D9" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>